<commit_message>
Revert "Update latest Documents"
This reverts commit 0775c26a472c22a90e36af39bde627b92e547f0f.
</commit_message>
<xml_diff>
--- a/Sage.CA.SBS.ERP.Sage300.SC/Source/ENG/Docs/Implementation Checklist.xlsx
+++ b/Sage.CA.SBS.ERP.Sage300.SC/Source/ENG/Docs/Implementation Checklist.xlsx
@@ -1,31 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evelyn.peh\Desktop\Doc2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019830AF-2248-4CAA-A084-DD03571983A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="15315" windowHeight="8775"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -125,6 +111,9 @@
     <t>Failure</t>
   </si>
   <si>
+    <t>Are you able to received threshold reached alert</t>
+  </si>
+  <si>
     <t>Are you able to receive Standard Chartered Loan campaign email</t>
   </si>
   <si>
@@ -380,6 +369,31 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Can you received test emaill during Settings/Options</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Webdings"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Cash Management Options Report (SCOPT)</t>
     </r>
   </si>
@@ -989,40 +1003,12 @@
   </si>
   <si>
     <t>Activation and configuration</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Webdings"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Can you receive test emaill during Settings/Options</t>
-    </r>
-  </si>
-  <si>
-    <t>Are you able to receive threshold reached alert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1215,6 +1201,9 @@
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1248,6 +1237,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1266,32 +1258,26 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1317,22 +1303,19 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{20DD1B9E-87C4-11D1-8BE3-0000F8754DA1}" ax:license="651A8940-87C5-11d1-8BE3-0000F8754DA1" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="_ExtentX" ax:value="4614"/>
-  <ax:ocxPr ax:name="_ExtentY" ax:value="720"/>
+  <ax:ocxPr ax:name="_ExtentX" ax:value="3519"/>
+  <ax:ocxPr ax:name="_ExtentY" ax:value="556"/>
   <ax:ocxPr ax:name="_Version" ax:value="393216"/>
   <ax:ocxPr ax:name="Font">
     <ax:font ax:persistence="persistPropertyBag">
       <ax:ocxPr ax:name="Name" ax:value="Calibri"/>
-      <ax:ocxPr ax:name="Size" ax:value="9.6"/>
+      <ax:ocxPr ax:name="Size" ax:value="9.75"/>
       <ax:ocxPr ax:name="Charset" ax:value="0"/>
       <ax:ocxPr ax:name="Weight" ax:value="400"/>
       <ax:ocxPr ax:name="Underline" ax:value="0"/>
@@ -1340,7 +1323,7 @@
       <ax:ocxPr ax:name="Strikethrough" ax:value="0"/>
     </ax:font>
   </ax:ocxPr>
-  <ax:ocxPr ax:name="Format" ax:value="1365114881"/>
+  <ax:ocxPr ax:name="Format" ax:value="563675137"/>
   <ax:ocxPr ax:name="CurrentDate" ax:value="43778"/>
 </ax:ocx>
 </file>
@@ -1352,15 +1335,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>22860</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1287780</xdr:colOff>
+          <xdr:colOff>1289050</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:rowOff>184150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1369,14 +1352,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1384,20 +1364,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1451,7 +1417,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1484,26 +1450,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1536,23 +1485,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1728,56 +1660,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:M68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
+      <pane ySplit="5" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="70.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="56.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="70.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="56.140625" style="2" customWidth="1"/>
     <col min="6" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-    </row>
-    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="B5" s="13" t="s">
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="J5" t="s">
@@ -1790,15 +1722,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="17" t="s">
+    <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
       <c r="J6" t="s">
         <v>6</v>
       </c>
@@ -1809,15 +1741,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="8">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="9">
         <v>1</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11" t="str">
+      <c r="D7" s="11"/>
+      <c r="E7" s="12" t="str">
         <f>IF(D7="Yes", L$5,IF(D7="","",L$6))</f>
         <v/>
       </c>
@@ -1825,15 +1757,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="8">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="9">
         <v>2</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11" t="str">
+      <c r="D8" s="11"/>
+      <c r="E8" s="12" t="str">
         <f>IF(D8="Yes", L$5,IF(D8="","",L$6))</f>
         <v/>
       </c>
@@ -1844,15 +1776,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="8">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="9">
         <v>3</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11" t="str">
+      <c r="D9" s="11"/>
+      <c r="E9" s="12" t="str">
         <f>IF(D9="Yes", L$5,IF(D9="","",L$6))</f>
         <v/>
       </c>
@@ -1863,15 +1795,15 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="8">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
         <v>4</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11" t="str">
+      <c r="C10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12" t="str">
         <f>IF(D10="Yes", L$5,IF(D10="","",L$6))</f>
         <v/>
       </c>
@@ -1879,609 +1811,609 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M11">
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="18" t="s">
+    <row r="12" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="8">
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="9">
         <v>1</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11" t="str">
+      <c r="D13" s="11"/>
+      <c r="E13" s="12" t="str">
         <f t="shared" ref="E13:E14" si="0">IF(D13="Yes", L$5,IF(D13="","",L$6))</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="8">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="9">
         <v>2</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11" t="str">
+      <c r="D14" s="11"/>
+      <c r="E14" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="21">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="13">
         <v>3</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="21"/>
-      <c r="C16" s="12" t="s">
+    <row r="16" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="13"/>
+      <c r="C16" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12" t="str">
+        <f t="shared" ref="E16:E17" si="1">IF(D16="Yes", L$5,IF(D16="","",L$6))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="13"/>
+      <c r="C17" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
+      <c r="C18" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12" t="str">
+        <f t="shared" ref="E19:E27" si="2">IF(D19="Yes", L$5,IF(D19="","",L$6))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="13"/>
+      <c r="C21" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="13"/>
+      <c r="C22" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="9">
+        <v>4</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="9">
+        <v>5</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="9">
+        <v>6</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="9">
+        <v>7</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="13">
+        <v>8</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="13"/>
+      <c r="C29" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12" t="str">
+        <f>IF(D29="Yes", L$5,IF(D29="","",L$6))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="13"/>
+      <c r="C30" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="12" t="str">
+        <f>IF(D30="Yes", L$5,IF(D30="","",L$6))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="13"/>
+      <c r="C31" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="12" t="str">
+        <f t="shared" ref="E31:E34" si="3">IF(D31="Yes", L$5,IF(D31="","",L$6))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="13"/>
+      <c r="C32" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="13"/>
+      <c r="C33" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="13"/>
+      <c r="C34" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="11"/>
+      <c r="E34" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="13">
+        <v>9</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="13"/>
+      <c r="C36" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="11"/>
+      <c r="E36" s="12" t="str">
+        <f t="shared" ref="E36:E40" si="4">IF(D36="Yes", L$5,IF(D36="","",L$6))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="13"/>
+      <c r="C37" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="11"/>
+      <c r="E37" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="13"/>
+      <c r="C38" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="13"/>
+      <c r="C39" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="9">
+        <v>10</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="11"/>
+      <c r="E40" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="9">
+        <v>11</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="11"/>
+      <c r="E41" s="12"/>
+    </row>
+    <row r="43" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="9">
+        <v>1</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="11"/>
+      <c r="E44" s="12" t="str">
+        <f t="shared" ref="E44" si="5">IF(D44="Yes", L$5,IF(D44="","",L$6))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="13">
+        <v>2</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11" t="str">
-        <f t="shared" ref="E16:E17" si="1">IF(D16="Yes", L$5,IF(D16="","",L$6))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="21"/>
-      <c r="C17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="21"/>
-      <c r="C18" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="21"/>
-      <c r="C19" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11" t="str">
-        <f t="shared" ref="E19:E27" si="2">IF(D19="Yes", L$5,IF(D19="","",L$6))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="21"/>
-      <c r="C20" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="21"/>
-      <c r="C21" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="21"/>
-      <c r="C22" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="21"/>
-      <c r="C23" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="8">
+    </row>
+    <row r="46" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="13"/>
+      <c r="C46" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="11"/>
+      <c r="E46" s="12" t="str">
+        <f t="shared" ref="E46:E47" si="6">IF(D46="Yes", L$5,IF(D46="","",L$6))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="13"/>
+      <c r="C47" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" s="11"/>
+      <c r="E47" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="9">
+        <v>1</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="11"/>
+      <c r="E50" s="12" t="str">
+        <f t="shared" ref="E50" si="7">IF(D50="Yes", L$5,IF(D50="","",L$6))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="13">
+        <v>2</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="13"/>
+      <c r="C52" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" s="11"/>
+      <c r="E52" s="12" t="str">
+        <f t="shared" ref="E52:E62" si="8">IF(D52="Yes", L$5,IF(D52="","",L$6))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="13"/>
+      <c r="C53" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" s="11"/>
+      <c r="E53" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="13"/>
+      <c r="C54" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" s="11"/>
+      <c r="E54" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="13"/>
+      <c r="C55" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="11"/>
+      <c r="E55" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B56" s="13"/>
+      <c r="C56" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D56" s="11"/>
+      <c r="E56" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="13"/>
+      <c r="C57" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D57" s="11"/>
+      <c r="E57" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="13"/>
+      <c r="C58" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D58" s="11"/>
+      <c r="E58" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="13"/>
+      <c r="C59" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" s="11"/>
+      <c r="E59" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B60" s="13"/>
+      <c r="C60" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D60" s="11"/>
+      <c r="E60" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="9">
+        <v>3</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="11"/>
+      <c r="E61" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="9">
         <v>4</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="8">
-        <v>5</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="8">
-        <v>6</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="8">
-        <v>7</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="21">
-        <v>8</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="21"/>
-      <c r="C29" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="11" t="str">
-        <f>IF(D29="Yes", L$5,IF(D29="","",L$6))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="21"/>
-      <c r="C30" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="11" t="str">
-        <f>IF(D30="Yes", L$5,IF(D30="","",L$6))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="21"/>
-      <c r="C31" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="11" t="str">
-        <f t="shared" ref="E31:E34" si="3">IF(D31="Yes", L$5,IF(D31="","",L$6))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="21"/>
-      <c r="C32" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="21"/>
-      <c r="C33" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="21"/>
-      <c r="C34" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="21">
-        <v>9</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="21"/>
-      <c r="C36" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11" t="str">
-        <f t="shared" ref="E36:E40" si="4">IF(D36="Yes", L$5,IF(D36="","",L$6))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="21"/>
-      <c r="C37" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B38" s="21"/>
-      <c r="C38" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B39" s="21"/>
-      <c r="C39" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="8">
-        <v>10</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="8">
-        <v>11</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
-    </row>
-    <row r="43" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B43" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="8">
-        <v>1</v>
-      </c>
-      <c r="C44" s="9" t="s">
+      <c r="C62" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="11" t="str">
-        <f t="shared" ref="E44" si="5">IF(D44="Yes", L$5,IF(D44="","",L$6))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B45" s="21">
-        <v>2</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="21"/>
-      <c r="C46" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="11" t="str">
-        <f t="shared" ref="E46:E47" si="6">IF(D46="Yes", L$5,IF(D46="","",L$6))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="21"/>
-      <c r="C47" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="11" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B49" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="8">
-        <v>1</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="11" t="str">
-        <f t="shared" ref="E50" si="7">IF(D50="Yes", L$5,IF(D50="","",L$6))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="21">
-        <v>2</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="21"/>
-      <c r="C52" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D52" s="10"/>
-      <c r="E52" s="11" t="str">
-        <f t="shared" ref="E52:E62" si="8">IF(D52="Yes", L$5,IF(D52="","",L$6))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="21"/>
-      <c r="C53" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D53" s="10"/>
-      <c r="E53" s="11" t="str">
+      <c r="D62" s="11"/>
+      <c r="E62" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="21"/>
-      <c r="C54" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D54" s="10"/>
-      <c r="E54" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="21"/>
-      <c r="C55" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="21"/>
-      <c r="C56" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D56" s="10"/>
-      <c r="E56" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="21"/>
-      <c r="C57" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D57" s="10"/>
-      <c r="E57" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" s="21"/>
-      <c r="C58" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D58" s="10"/>
-      <c r="E58" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="21"/>
-      <c r="C59" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D59" s="10"/>
-      <c r="E59" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="21"/>
-      <c r="C60" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D60" s="10"/>
-      <c r="E60" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B61" s="8">
-        <v>3</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D61" s="10"/>
-      <c r="E61" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="8">
-        <v>4</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="2:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="20" t="s">
-        <v>70</v>
+    <row r="63" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="26" t="s">
+        <v>72</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D64" s="27"/>
       <c r="E64" s="28"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C65" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D65" s="8" t="str">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" s="9" t="str">
         <f>IF((COUNTIF(D7:D10,"=Yes")=4)=FALSE,"INCOMPLETE","COMPLETED")</f>
         <v>INCOMPLETE</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C66" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D66" s="8" t="str">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D66" s="9" t="str">
         <f>IF((COUNTIF(D13:D41,"=Yes")=25)=FALSE,"INCOMPLETE","COMPLETED")</f>
         <v>INCOMPLETE</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C67" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D67" s="8" t="str">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C67" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" s="9" t="str">
         <f>IF((COUNTIF(D44:D47,"=Yes")=3)=FALSE,"INCOMPLETE","COMPLETED")</f>
         <v>INCOMPLETE</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C68" s="9" t="s">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D68" s="8" t="str">
+      <c r="D68" s="9" t="str">
         <f>IF((COUNTIF(D50:D62,"=Yes")=12)=FALSE,"INCOMPLETE","COMPLETED")</f>
         <v>INCOMPLETE</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="B15:B23"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="B45:B47"/>
     <mergeCell ref="B51:B60"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="B15:B23"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="B45:B47"/>
   </mergeCells>
   <conditionalFormatting sqref="D65">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
@@ -2489,21 +2421,21 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D13:D14 D61:D62 D50 D16:D17 D19:D27 D29:D34 D44:D47 D36:D41" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D13:D14 D61:D62 D50 D16:D17 D19:D27 D29:D34 D44:D47 D36:D41">
       <formula1>$K$5:$K$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9">
       <formula1>$J$5:$J$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D52:D60" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D52:D60">
       <formula1>$K$8:$K$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10">
       <formula1>$M$8:$M$11</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <controls>
@@ -2514,15 +2446,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>22860</xdr:colOff>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>1</xdr:row>
-                <xdr:rowOff>182880</xdr:rowOff>
+                <xdr:rowOff>180975</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>1287780</xdr:colOff>
+                <xdr:colOff>1285875</xdr:colOff>
                 <xdr:row>2</xdr:row>
-                <xdr:rowOff>182880</xdr:rowOff>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -2537,26 +2469,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>